<commit_message>
GDE-9501: Add TL Base Rate for PT Health
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Base_Rate/BaseRates_Files_27DEC2019/TL_Transformed_Data_BaseRate.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Base_Rate/BaseRates_Files_27DEC2019/TL_Transformed_Data_BaseRate.xlsx
@@ -83,6 +83,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -504,14 +572,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>0.93</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>null</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.8496</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>null</t>
@@ -524,7 +592,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2019-12-16</t>
+          <t>2020-11-25</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -539,7 +607,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>001M</t>
+          <t>003M</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">

</xml_diff>